<commit_message>
refactor troop initialization and enhance attack logic with error handling
</commit_message>
<xml_diff>
--- a/Risiko/RisiKo.xlsx
+++ b/Risiko/RisiKo.xlsx
@@ -8,9 +8,9 @@
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Giocatori" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Matteo" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Agata" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Asia" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Agata" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Asia" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Francesca" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -450,7 +450,7 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>Matteo</t>
+          <t>Agata</t>
         </is>
       </c>
     </row>
@@ -484,7 +484,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Conquistare l'Asia e il Sud America.</t>
+          <t>Conquistare 18 territori a scelta.</t>
         </is>
       </c>
     </row>
@@ -520,12 +520,12 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>giappone</t>
+          <t>scandinavia</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>asia</t>
+          <t>europa</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -534,13 +534,13 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>siam</t>
+          <t>kamchatka</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -550,17 +550,17 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>cavallo</t>
+          <t>cannone</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>scandinavia</t>
+          <t>europa meridionale</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -574,38 +574,38 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>irkutsk</t>
+          <t>alberta</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>asia</t>
+          <t>america del nord</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>fante</t>
+          <t>cavallo</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>india</t>
+          <t>australia orientale</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>asia</t>
+          <t>oceania</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -614,98 +614,98 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>egitto</t>
+          <t>america centrale</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>africa</t>
+          <t>america del nord</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>fante</t>
+          <t>cavallo</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>gran bretagna</t>
+          <t>territori del nord-ovest</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>europa</t>
+          <t>america del nord</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>cavallo</t>
+          <t>cannone</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>nuova guinea</t>
+          <t>venezuela</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>oceania</t>
+          <t>america del sud</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>cavallo</t>
+          <t>cannone</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>africa orientale</t>
+          <t>europa occidentale</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>africa</t>
+          <t>europa</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>cannone</t>
+          <t>fante</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>europa meridionale</t>
+          <t>giappone</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>europa</t>
+          <t>asia</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -714,13 +714,13 @@
         </is>
       </c>
       <c r="D18" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>argentina</t>
+          <t>brasile</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -730,62 +730,62 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>cannone</t>
+          <t>cavallo</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>alberta</t>
+          <t>argentina</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>america del nord</t>
+          <t>america del sud</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>cavallo</t>
+          <t>cannone</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>indonesia</t>
+          <t>siberia</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>oceania</t>
+          <t>asia</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>fante</t>
+          <t>cannone</t>
         </is>
       </c>
       <c r="D21" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>groenlandia</t>
+          <t>perù</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>america del nord</t>
+          <t>america del sud</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -794,7 +794,7 @@
         </is>
       </c>
       <c r="D22" t="n">
-        <v>5</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -824,7 +824,7 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>Agata</t>
+          <t>Asia</t>
         </is>
       </c>
     </row>
@@ -858,7 +858,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Conquistare il Nord America e l'Europa.</t>
+          <t>Conquistare il Nord America e l'Africa.</t>
         </is>
       </c>
     </row>
@@ -894,87 +894,75 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>congo</t>
+          <t>mongolia</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>africa</t>
+          <t>asia</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
           <t>cavallo</t>
         </is>
-      </c>
-      <c r="D9" t="n">
-        <v>9</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>stati uniti orientali</t>
+          <t>irkutsk</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>america del nord</t>
+          <t>asia</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
           <t>fante</t>
         </is>
-      </c>
-      <c r="D10" t="n">
-        <v>8</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>australia orientale</t>
+          <t>africa del sud</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>oceania</t>
+          <t>africa</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
           <t>fante</t>
         </is>
-      </c>
-      <c r="D11" t="n">
-        <v>5</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>perù</t>
+          <t>australia occidentale</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>america del sud</t>
+          <t>oceania</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>fante</t>
-        </is>
-      </c>
-      <c r="D12" t="n">
-        <v>5</v>
+          <t>cannone</t>
+        </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>siberia</t>
+          <t>india</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -984,51 +972,42 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>cannone</t>
-        </is>
-      </c>
-      <c r="D13" t="n">
-        <v>6</v>
+          <t>fante</t>
+        </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>europa occidentale</t>
+          <t>africa orientale</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>europa</t>
+          <t>africa</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>fante</t>
-        </is>
-      </c>
-      <c r="D14" t="n">
-        <v>6</v>
+          <t>cannone</t>
+        </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>quebec</t>
+          <t>europa settentrionale</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>america del nord</t>
+          <t>europa</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>fante</t>
-        </is>
-      </c>
-      <c r="D15" t="n">
-        <v>5</v>
+          <t>cavallo</t>
+        </is>
       </c>
     </row>
     <row r="16">
@@ -1047,54 +1026,45 @@
           <t>cavallo</t>
         </is>
       </c>
-      <c r="D16" t="n">
-        <v>7</v>
-      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>mongolia</t>
+          <t>groenlandia</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>asia</t>
+          <t>america del nord</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>cavallo</t>
-        </is>
-      </c>
-      <c r="D17" t="n">
-        <v>5</v>
+          <t>fante</t>
+        </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>brasile</t>
+          <t>ontario</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>america del sud</t>
+          <t>america del nord</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>cavallo</t>
-        </is>
-      </c>
-      <c r="D18" t="n">
-        <v>8</v>
+          <t>cannone</t>
+        </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>territori del nord-ovest</t>
+          <t>stati uniti occidentali</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -1106,55 +1076,46 @@
         <is>
           <t>cannone</t>
         </is>
-      </c>
-      <c r="D19" t="n">
-        <v>4</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>islanda</t>
+          <t>medio oriente</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>europa</t>
+          <t>asia</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>fante</t>
-        </is>
-      </c>
-      <c r="D20" t="n">
-        <v>5</v>
+          <t>cannone</t>
+        </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>africa del sud</t>
+          <t>ucraina</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>africa</t>
+          <t>europa</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
           <t>fante</t>
         </is>
-      </c>
-      <c r="D21" t="n">
-        <v>8</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>urali</t>
+          <t>jacuzia</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -1164,11 +1125,8 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>cavallo</t>
-        </is>
-      </c>
-      <c r="D22" t="n">
-        <v>3</v>
+          <t>fante</t>
+        </is>
       </c>
     </row>
   </sheetData>
@@ -1198,7 +1156,7 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>Asia</t>
+          <t>Francesca</t>
         </is>
       </c>
     </row>
@@ -1232,7 +1190,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Conquistare 24 territori occupandoli con almeno 2 armate ciascuno.</t>
+          <t>Conquistare l'Africa e l'Europa.</t>
         </is>
       </c>
     </row>
@@ -1268,227 +1226,194 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>australia occidentale</t>
+          <t>congo</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>oceania</t>
+          <t>africa</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>cannone</t>
-        </is>
-      </c>
-      <c r="D9" t="n">
-        <v>5</v>
+          <t>cavallo</t>
+        </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>venezuela</t>
+          <t>afghanistan</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>america del sud</t>
+          <t>asia</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>cannone</t>
-        </is>
-      </c>
-      <c r="D10" t="n">
-        <v>9</v>
+          <t>fante</t>
+        </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>jacuzia</t>
+          <t>africa del nord</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>asia</t>
+          <t>africa</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>fante</t>
-        </is>
-      </c>
-      <c r="D11" t="n">
-        <v>4</v>
+          <t>cannone</t>
+        </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>stati uniti occidentali</t>
+          <t>gran bretagna</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>america del nord</t>
+          <t>europa</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>cannone</t>
-        </is>
-      </c>
-      <c r="D12" t="n">
-        <v>5</v>
+          <t>cavallo</t>
+        </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>medio oriente</t>
+          <t>indonesia</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>asia</t>
+          <t>oceania</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>cannone</t>
-        </is>
-      </c>
-      <c r="D13" t="n">
-        <v>6</v>
+          <t>fante</t>
+        </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>ontario</t>
+          <t>nuova guinea</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>america del nord</t>
+          <t>oceania</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>cannone</t>
-        </is>
-      </c>
-      <c r="D14" t="n">
-        <v>4</v>
+          <t>cavallo</t>
+        </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>afghanistan</t>
+          <t>alaska</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>asia</t>
+          <t>america del nord</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>fante</t>
-        </is>
-      </c>
-      <c r="D15" t="n">
-        <v>6</v>
+          <t>cavallo</t>
+        </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>ucraina</t>
+          <t>cina</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>europa</t>
+          <t>asia</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>fante</t>
-        </is>
-      </c>
-      <c r="D16" t="n">
-        <v>5</v>
+          <t>cannone</t>
+        </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>africa del nord</t>
+          <t>islanda</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>africa</t>
+          <t>europa</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>cannone</t>
-        </is>
-      </c>
-      <c r="D17" t="n">
-        <v>5</v>
+          <t>fante</t>
+        </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>kamchatka</t>
+          <t>madagascar</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>asia</t>
+          <t>africa</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>cannone</t>
-        </is>
-      </c>
-      <c r="D18" t="n">
-        <v>4</v>
+          <t>cavallo</t>
+        </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>europa settentrionale</t>
+          <t>siam</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>europa</t>
+          <t>asia</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
           <t>cavallo</t>
         </is>
-      </c>
-      <c r="D19" t="n">
-        <v>5</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>madagascar</t>
+          <t>egitto</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -1498,51 +1423,42 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>cavallo</t>
-        </is>
-      </c>
-      <c r="D20" t="n">
-        <v>6</v>
+          <t>fante</t>
+        </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>cina</t>
+          <t>quebec</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>asia</t>
+          <t>america del nord</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>cannone</t>
-        </is>
-      </c>
-      <c r="D21" t="n">
-        <v>6</v>
+          <t>fante</t>
+        </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>alaska</t>
+          <t>urali</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>america del nord</t>
+          <t>asia</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
           <t>cavallo</t>
         </is>
-      </c>
-      <c r="D22" t="n">
-        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>